<commit_message>
Not sure what I chagned here
</commit_message>
<xml_diff>
--- a/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A1/K4S_DA_A1/summary_table.xlsx
+++ b/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A1/K4S_DA_A1/summary_table.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/University/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoestarkey/Desktop/Honours/Data_Analysis/K_axis_midoc/K4S_key_scripts/K4S_DA_Aims/K4S_DA_A1/K4S_DA_A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8D6908B-1F4A-5240-85A0-296277F4E486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D8788E-D887-DF4E-AA3E-71557CC0C970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8A1D5A3D-DB14-B841-8B04-959120807A9A}"/>
+    <workbookView xWindow="6680" yWindow="780" windowWidth="28800" windowHeight="18000" xr2:uid="{8A1D5A3D-DB14-B841-8B04-959120807A9A}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_table" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
   <si>
     <t>Group</t>
   </si>
@@ -261,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +446,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -632,18 +639,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -689,7 +696,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -714,6 +721,12 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -735,6 +748,23 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2994,7 +3024,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -9768,7 +9798,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{06E070C2-7A20-9340-AE27-D53A38EE6FA9}" name="Table1" displayName="Table1" ref="A2:D13" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{06E070C2-7A20-9340-AE27-D53A38EE6FA9}" name="Table1" displayName="Table1" ref="A2:D13" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A2:D13" xr:uid="{06E070C2-7A20-9340-AE27-D53A38EE6FA9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9778,21 +9808,34 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{37C5C9AD-D7E3-1043-83C6-F48981B7033E}" name="Group"/>
     <tableColumn id="2" xr3:uid="{6E1588EF-5E76-554B-AE2A-7B021CF01D90}" name="Number of entries"/>
-    <tableColumn id="3" xr3:uid="{FE2B909E-F8C9-F047-84C1-1640F5A25506}" name="Summed biomass" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{FA41EF5F-0BD8-9B48-B419-354565D1C30C}" name="Percentage of total" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{FE2B909E-F8C9-F047-84C1-1640F5A25506}" name="Summed biomass" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{FA41EF5F-0BD8-9B48-B419-354565D1C30C}" name="Percentage of total" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9122DA47-57A7-6243-8A14-29A7EBA63DE5}" name="Table13" displayName="Table13" ref="A17:D27" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9122DA47-57A7-6243-8A14-29A7EBA63DE5}" name="Table13" displayName="Table13" ref="A17:D27" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A17:D27" xr:uid="{9122DA47-57A7-6243-8A14-29A7EBA63DE5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{290118BD-8A3D-744A-98B4-D539855C262B}" name="Group"/>
     <tableColumn id="2" xr3:uid="{C59B9035-C46C-744A-845B-E59EDD6834FB}" name="Number of entries"/>
-    <tableColumn id="3" xr3:uid="{E47EC7AD-B8B0-7E41-BAC1-85F8E9DEE39B}" name="Summed biomass" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{F5E65C62-75F8-C741-B3C7-8C04C2BDCA76}" name="Percentage of total" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E47EC7AD-B8B0-7E41-BAC1-85F8E9DEE39B}" name="Summed biomass" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{F5E65C62-75F8-C741-B3C7-8C04C2BDCA76}" name="Percentage of total" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8EE3EA05-3583-4F45-8B7E-F511A3FF1555}" name="Table134" displayName="Table134" ref="E9:H19" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="E9:H19" xr:uid="{8EE3EA05-3583-4F45-8B7E-F511A3FF1555}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{348A4A0D-0FDB-4344-8563-E55249A40C40}" name="Group"/>
+    <tableColumn id="2" xr3:uid="{C0E5C809-39B3-2D47-A8B3-70605089D741}" name="Number of entries"/>
+    <tableColumn id="3" xr3:uid="{BC272797-127B-3245-9917-DBAE3C30EE29}" name="Summed biomass" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BB56FB3C-7A75-5D4F-B8AE-BA356D56441F}" name="Percentage of total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10117,8 +10160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8CFA90-3A7D-3B4F-94D9-C338E93F98DD}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="X9" sqref="W9:X9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10129,12 +10172,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -10305,12 +10348,12 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -10400,7 +10443,7 @@
         <f>(Table13[[#This Row],[Summed biomass]]/$C$27)*100</f>
         <v>1.9916676846493238</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -10416,7 +10459,7 @@
         <f>(Table13[[#This Row],[Summed biomass]]/$C$27)*100</f>
         <v>1.4114432459136887</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -10432,7 +10475,7 @@
         <f>(Table13[[#This Row],[Summed biomass]]/$C$27)*100</f>
         <v>0.7275287547417344</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -10448,7 +10491,7 @@
         <f>(Table13[[#This Row],[Summed biomass]]/$C$27)*100</f>
         <v>9.5149643228132632</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -10464,7 +10507,7 @@
         <f>(Table13[[#This Row],[Summed biomass]]/$C$27)*100</f>
         <v>6.652236719593752</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -10480,52 +10523,52 @@
       <c r="D27" s="1">
         <v>100</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E28" s="5"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E29" s="5"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E30" s="5"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="5"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33">
         <v>202</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="1">
         <v>2.0414160000000001E-2</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="1">
         <v>0.63717051000000002</v>
       </c>
     </row>
@@ -10536,24 +10579,24 @@
       <c r="B34" s="3">
         <v>370</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <v>2.2700785799999998</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>70.854107999999997</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35">
         <v>229</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="1">
         <v>0.37112323000000003</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="1">
         <v>11.5835662</v>
       </c>
     </row>
@@ -10564,24 +10607,24 @@
       <c r="B36" s="3">
         <v>285</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="6">
         <v>0.11799488</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>3.68287772</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37">
         <v>42</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="1">
         <v>2.055384E-2</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="1">
         <v>0.64153017000000001</v>
       </c>
     </row>
@@ -10592,24 +10635,24 @@
       <c r="B38" s="3">
         <v>8</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>1.4565969999999999E-2</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="6">
         <v>0.45463579999999998</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39">
         <v>113</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="1">
         <v>6.8650509999999998E-2</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="1">
         <v>2.14273224</v>
       </c>
     </row>
@@ -10620,46 +10663,46 @@
       <c r="B40" s="3">
         <v>73</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <v>0.32049517</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="6">
         <v>10.0033539</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41">
         <v>1323</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="1">
         <v>3.2038771499999998</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10670,25 +10713,25 @@
       <c r="B45" s="3">
         <v>202</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="6">
         <v>2.0414160000000001E-2</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="6">
         <f>(C45/$C$52)*100</f>
         <v>2.1861436035143198</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46">
         <v>229</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="1">
         <v>0.37112323000000003</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="1">
         <f t="shared" ref="D46:D51" si="0">(C46/$C$52)*100</f>
         <v>39.743426885067706</v>
       </c>
@@ -10700,25 +10743,25 @@
       <c r="B47" s="3">
         <v>285</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="6">
         <v>0.11799488</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="6">
         <f t="shared" si="0"/>
         <v>12.636020887434981</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48">
         <v>42</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="1">
         <v>2.055384E-2</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D48" s="1">
         <f t="shared" si="0"/>
         <v>2.2011018745643596</v>
       </c>
@@ -10730,25 +10773,25 @@
       <c r="B49" s="3">
         <v>8</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="6">
         <v>1.4565969999999999E-2</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="6">
         <f t="shared" si="0"/>
         <v>1.5598634548020331</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="A50" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50">
         <v>113</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="1">
         <v>6.8650509999999998E-2</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D50" s="1">
         <f t="shared" si="0"/>
         <v>7.3517535531462395</v>
       </c>
@@ -10760,62 +10803,62 @@
       <c r="B51" s="3">
         <v>73</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="6">
         <v>0.32049517</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="6">
         <f t="shared" si="0"/>
         <v>34.321689741470358</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="A52" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52">
         <v>1323</v>
       </c>
-      <c r="C52" s="8">
+      <c r="C52" s="1">
         <f>SUM(C45:C51)</f>
         <v>0.93379776000000003</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60">
         <v>202</v>
       </c>
-      <c r="C60" s="8">
+      <c r="C60" s="1">
         <v>2.0414160247913201E-2</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D60" s="1">
         <v>0.63717050524922803</v>
       </c>
     </row>
@@ -10826,24 +10869,24 @@
       <c r="B61" s="3">
         <v>206</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="6">
         <v>2.17188496733591</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D61" s="6">
         <v>67.789271034162894</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62">
         <v>229</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C62" s="1">
         <v>0.37112322982056301</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D62" s="1">
         <v>11.583566161075099</v>
       </c>
     </row>
@@ -10854,24 +10897,24 @@
       <c r="B63" s="3">
         <v>146</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="6">
         <v>0.110486843837863</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="6">
         <v>3.4485355878775601</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="A64" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64">
         <v>73</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C64" s="1">
         <v>0.32049517132628502</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D64" s="1">
         <v>10.003353934912999</v>
       </c>
     </row>
@@ -10882,46 +10925,46 @@
       <c r="B65" s="3">
         <v>467</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="6">
         <v>0.20947278115003801</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="6">
         <v>6.5381027767220603</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66">
         <v>1323</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C66" s="1">
         <v>3.2038771537185702</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D66" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -10932,25 +10975,25 @@
       <c r="B75" s="3">
         <v>202</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="6">
         <v>2.0414160247913201E-2</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D75" s="6">
         <f>(C75/$C$80)*100</f>
         <v>1.9781312801862281</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="A76" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76">
         <v>229</v>
       </c>
-      <c r="C76" s="8">
+      <c r="C76" s="1">
         <v>0.37112322982056301</v>
       </c>
-      <c r="D76" s="8">
+      <c r="D76" s="1">
         <f t="shared" ref="D76:D79" si="1">(C76/$C$80)*100</f>
         <v>35.961825556201518</v>
       </c>
@@ -10962,25 +11005,25 @@
       <c r="B77" s="3">
         <v>146</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="6">
         <v>0.110486843837863</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="6">
         <f t="shared" si="1"/>
         <v>10.706170579172829</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="A78" t="s">
         <v>13</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B78">
         <v>73</v>
       </c>
-      <c r="C78" s="8">
+      <c r="C78" s="1">
         <v>0.32049517132628502</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D78" s="1">
         <f t="shared" si="1"/>
         <v>31.055968790779737</v>
       </c>
@@ -10992,26 +11035,26 @@
       <c r="B79" s="3">
         <v>467</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="6">
         <v>0.20947278115003801</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D79" s="6">
         <f t="shared" si="1"/>
         <v>20.297903793659692</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+      <c r="A80" t="s">
         <v>14</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B80">
         <v>1323</v>
       </c>
-      <c r="C80" s="8">
+      <c r="C80" s="1">
         <f>SUM(C75:C79)</f>
         <v>1.0319921863826622</v>
       </c>
-      <c r="D80" s="8">
+      <c r="D80" s="1">
         <f>SUM(D75:D79)</f>
         <v>100</v>
       </c>
@@ -11035,6 +11078,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7D49C1-A878-DC45-9D67-B6954EF62952}">
+  <dimension ref="E8:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>202</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.0414160247913201E-2</v>
+      </c>
+      <c r="H10" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/G19)*100</f>
+        <v>1.9781328454239098</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>229</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.37112322982056301</v>
+      </c>
+      <c r="H11" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>35.961854011746929</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>146</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.110486843837863</v>
+      </c>
+      <c r="H12" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>10.70617905065386</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="9">
+        <v>73</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.32049517132628502</v>
+      </c>
+      <c r="H13" s="10">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>31.055993364463539</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2.0553838620635499E-2</v>
+      </c>
+      <c r="H14" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>1.9916676846493238</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.4565972487425201E-2</v>
+      </c>
+      <c r="H15" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>1.4114432459136887</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>139</v>
+      </c>
+      <c r="G16" s="1">
+        <v>7.5080339617331297E-3</v>
+      </c>
+      <c r="H16" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>0.7275287547417344</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>164</v>
+      </c>
+      <c r="G17" s="1">
+        <v>9.8193610650785995E-2</v>
+      </c>
+      <c r="H17" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>9.5149643228132632</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>113</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6.8650508844737196E-2</v>
+      </c>
+      <c r="H18" s="1">
+        <f>(Table134[[#This Row],[Summed biomass]]/$G$19)*100</f>
+        <v>6.652236719593752</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>1323</v>
+      </c>
+      <c r="G19" s="1">
+        <f>SUM(G10:G18)</f>
+        <v>1.0319913697979413</v>
+      </c>
+      <c r="H19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E8:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4C70C4-DE9C-8B45-A946-5CC6F049409D}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>